<commit_message>
fitur excel rekap pembelian tanah
</commit_message>
<xml_diff>
--- a/application/controllers/file/laporan_rekap_evaluasi_pembelian.xlsx
+++ b/application/controllers/file/laporan_rekap_evaluasi_pembelian.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landargopuro\application\controllers\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroza\Documents\Project\landargopuro\application\controllers\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8DF30A-6C15-431A-B1FB-2DB46C8D6D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976D2191-293B-4A08-9189-C4E48D94BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F54AB4D7-7B2D-48B6-BA0E-3BB89B47F765}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>PT. GUNUNG BATU UTAMA</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>TAHUN 2020</t>
-  </si>
-  <si>
-    <t>I.</t>
-  </si>
-  <si>
-    <t>IP PROYEK - DALAM IJIN</t>
   </si>
   <si>
     <t>No</t>
@@ -334,9 +328,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,10 +337,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -669,14 +663,14 @@
   <dimension ref="A1:BD38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.54296875" style="1" customWidth="1"/>
@@ -962,12 +956,8 @@
       <c r="BB4" s="4"/>
     </row>
     <row r="5" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1077,18 +1067,18 @@
     </row>
     <row r="7" spans="1:54" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="22" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1096,12 +1086,12 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
@@ -1129,246 +1119,246 @@
     </row>
     <row r="8" spans="1:54" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R8" s="22"/>
       <c r="S8" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="T8" s="22"/>
       <c r="U8" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V8" s="22"/>
       <c r="W8" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X8" s="22"/>
       <c r="Y8" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z8" s="22"/>
       <c r="AA8" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AB8" s="22"/>
       <c r="AC8" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AD8" s="22"/>
       <c r="AE8" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AF8" s="22"/>
       <c r="AG8" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH8" s="22"/>
       <c r="AI8" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AJ8" s="22"/>
       <c r="AK8" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AL8" s="22"/>
     </row>
     <row r="9" spans="1:54" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="U9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="V9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="W9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="X9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL9" s="24" t="s">
-        <v>22</v>
+      <c r="O9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="W9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="X9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL9" s="21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:54" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
     </row>
     <row r="11" spans="1:54" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
@@ -1376,7 +1366,7 @@
     <row r="12" spans="1:54" s="10" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1411,7 +1401,7 @@
     <row r="13" spans="1:54" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
       <c r="B13" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1425,7 +1415,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -1440,7 +1430,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AB13" s="3"/>
       <c r="AC13" s="13"/>
@@ -1576,7 +1566,7 @@
     <row r="18" spans="1:56" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1590,7 +1580,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -1605,7 +1595,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB18" s="3"/>
       <c r="AC18" s="8"/>
@@ -1615,7 +1605,7 @@
     <row r="19" spans="1:56" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -1629,7 +1619,7 @@
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O19" s="18"/>
       <c r="P19" s="3"/>
@@ -1644,7 +1634,7 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AB19" s="3"/>
       <c r="AC19" s="11"/>
@@ -2213,6 +2203,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="AI8:AJ8"/>
     <mergeCell ref="AK8:AL8"/>
     <mergeCell ref="H8:I8"/>
@@ -2229,11 +2224,6 @@
     <mergeCell ref="AC8:AD8"/>
     <mergeCell ref="AE8:AF8"/>
     <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>